<commit_message>
tried to work with QUICKFS API but found out they use old data :(
</commit_message>
<xml_diff>
--- a/MyStocks.xlsx
+++ b/MyStocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian Mittmann\PycharmProjects\7 Hills\DipFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABDE4EE-D361-458E-AAE2-C93CDB9F2F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A205BE6F-F0CE-47A9-9A4C-3B6175035D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{B1263DE6-3D50-44DF-B2B7-F889FE7D3CCE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>O</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>MCD</t>
+  </si>
+  <si>
+    <t>BKNG</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E282671-166D-45DF-854B-9BF28CF3D7FB}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +650,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>